<commit_message>
Added 1 more excel scenario example
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestDataFiles/validateModelDropdownValues.xlsx
+++ b/src/test/resources/excelTestDataFiles/validateModelDropdownValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\carsautomation\src\test\resources\excelTestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E475985-97E3-4F49-A331-16E8DC95BDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0A1246-81FC-4826-B61F-1FE09881CF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{945B0ED5-0C35-4027-9BB3-A61CF9277062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{945B0ED5-0C35-4027-9BB3-A61CF9277062}"/>
   </bookViews>
   <sheets>
     <sheet name="carSearch" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>startingWithWord2</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>All models,Enclave,Encore,Encore GX,Envision,Envista,Skylark</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>All models,ILX,Integra,MDX,NSX,RDX,TLX</t>
   </si>
 </sst>
 </file>
@@ -104,12 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD46CEB8-EBB9-47BB-9A61-F104AF5D30BA}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +496,40 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>